<commit_message>
final gerbers sent to PCBway
</commit_message>
<xml_diff>
--- a/schematics/Connector.Filter.Board/gerber/ConnectorBoardPickAndPlace.xlsx
+++ b/schematics/Connector.Filter.Board/gerber/ConnectorBoardPickAndPlace.xlsx
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Connector.Board" localSheetId="1">Sheet2!$A$2:$F$122</definedName>
     <definedName name="Connector.Board_1" localSheetId="0">Sheet1!$A$2:$H$103</definedName>
+    <definedName name="Connector.Board_1" localSheetId="1">Sheet2!$A$123:$F$198</definedName>
     <definedName name="Connector.Board_2" localSheetId="0">Sheet1!$A$104:$H$183</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -54,11 +57,35 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="Connector.Board2" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\Jimbles\Parallel-CS\schematics\Connector.Filter.Board\gerber\Connector.Board.mnt" tab="0" space="1" consecutive="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="Connector.Board3" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\Jimbles\Parallel-CS\schematics\Connector.Filter.Board\gerber\Connector.Board.mnb" tab="0" space="1" consecutive="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="237">
   <si>
     <t>C1</t>
   </si>
@@ -692,6 +719,84 @@
   <si>
     <t>Side</t>
   </si>
+  <si>
+    <t>C87</t>
+  </si>
+  <si>
+    <t>C88</t>
+  </si>
+  <si>
+    <t>C92</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>C93</t>
+  </si>
+  <si>
+    <t>C94</t>
+  </si>
+  <si>
+    <t>LED3</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
+  </si>
+  <si>
+    <t>LED4</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>R67</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>R68</t>
+  </si>
+  <si>
+    <t>R69</t>
+  </si>
+  <si>
+    <t>U25</t>
+  </si>
+  <si>
+    <t>U27</t>
+  </si>
+  <si>
+    <t>MCP73831</t>
+  </si>
+  <si>
+    <t>SOT23-5</t>
+  </si>
+  <si>
+    <t>U28</t>
+  </si>
+  <si>
+    <t>LTC1044ACS8PBF</t>
+  </si>
+  <si>
+    <t>SOIC127P600X175-8N</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>MOLEX_47346-0001</t>
+  </si>
+  <si>
+    <t>C89</t>
+  </si>
+  <si>
+    <t>C90</t>
+  </si>
+  <si>
+    <t>U26</t>
+  </si>
 </sst>
 </file>
 
@@ -755,11 +860,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Connector.Board_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Connector.Board_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Connector.Board_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Connector.Board_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Connector.Board" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1027,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21632,4 +21745,4578 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G198"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K143" sqref="K143"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>129.54</v>
+      </c>
+      <c r="C2">
+        <v>62.48</v>
+      </c>
+      <c r="D2">
+        <v>180</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>129.54</v>
+      </c>
+      <c r="C3">
+        <v>38.1</v>
+      </c>
+      <c r="D3">
+        <v>180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>129.41</v>
+      </c>
+      <c r="C4">
+        <v>87</v>
+      </c>
+      <c r="D4">
+        <v>180</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>129.54</v>
+      </c>
+      <c r="C5">
+        <v>61.34</v>
+      </c>
+      <c r="D5">
+        <v>180</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>129.54</v>
+      </c>
+      <c r="C6">
+        <v>36.83</v>
+      </c>
+      <c r="D6">
+        <v>180</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>129.41</v>
+      </c>
+      <c r="C7">
+        <v>85.73</v>
+      </c>
+      <c r="D7">
+        <v>180</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>129.54</v>
+      </c>
+      <c r="C8">
+        <v>48.9</v>
+      </c>
+      <c r="D8">
+        <v>180</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>129.54</v>
+      </c>
+      <c r="C9">
+        <v>24.51</v>
+      </c>
+      <c r="D9">
+        <v>180</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>129.41</v>
+      </c>
+      <c r="C10">
+        <v>73.28</v>
+      </c>
+      <c r="D10">
+        <v>180</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>129.54</v>
+      </c>
+      <c r="C11">
+        <v>47.62</v>
+      </c>
+      <c r="D11">
+        <v>180</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>129.54</v>
+      </c>
+      <c r="C12">
+        <v>23.24</v>
+      </c>
+      <c r="D12">
+        <v>180</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>129.41</v>
+      </c>
+      <c r="C13">
+        <v>72.010000000000005</v>
+      </c>
+      <c r="D13">
+        <v>180</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>137.54</v>
+      </c>
+      <c r="C14">
+        <v>86.23</v>
+      </c>
+      <c r="D14">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>136.78</v>
+      </c>
+      <c r="C15">
+        <v>72.77</v>
+      </c>
+      <c r="D15">
+        <v>270</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>137.66999999999999</v>
+      </c>
+      <c r="C16">
+        <v>61.85</v>
+      </c>
+      <c r="D16">
+        <v>90</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>136.91</v>
+      </c>
+      <c r="C17">
+        <v>48.39</v>
+      </c>
+      <c r="D17">
+        <v>270</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>137.66999999999999</v>
+      </c>
+      <c r="C18">
+        <v>37.47</v>
+      </c>
+      <c r="D18">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>136.91</v>
+      </c>
+      <c r="C19">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>270</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C20">
+        <v>62.48</v>
+      </c>
+      <c r="D20">
+        <v>180</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C21">
+        <v>38.1</v>
+      </c>
+      <c r="D21">
+        <v>180</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>145.54</v>
+      </c>
+      <c r="C22">
+        <v>87</v>
+      </c>
+      <c r="D22">
+        <v>180</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C23">
+        <v>61.21</v>
+      </c>
+      <c r="D23">
+        <v>180</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C24">
+        <v>36.83</v>
+      </c>
+      <c r="D24">
+        <v>180</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>145.54</v>
+      </c>
+      <c r="C25">
+        <v>85.73</v>
+      </c>
+      <c r="D25">
+        <v>180</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C26">
+        <v>48.9</v>
+      </c>
+      <c r="D26">
+        <v>180</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C27">
+        <v>24.51</v>
+      </c>
+      <c r="D27">
+        <v>180</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>145.66999999999999</v>
+      </c>
+      <c r="C28">
+        <v>73.28</v>
+      </c>
+      <c r="D28">
+        <v>180</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C29">
+        <v>47.62</v>
+      </c>
+      <c r="D29">
+        <v>180</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C30">
+        <v>23.24</v>
+      </c>
+      <c r="D30">
+        <v>180</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>145.66999999999999</v>
+      </c>
+      <c r="C31">
+        <v>72.010000000000005</v>
+      </c>
+      <c r="D31">
+        <v>180</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="C32">
+        <v>86.23</v>
+      </c>
+      <c r="D32">
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>153.03</v>
+      </c>
+      <c r="C33">
+        <v>72.77</v>
+      </c>
+      <c r="D33">
+        <v>270</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>153.91999999999999</v>
+      </c>
+      <c r="C34">
+        <v>61.85</v>
+      </c>
+      <c r="D34">
+        <v>90</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>153.16</v>
+      </c>
+      <c r="C35">
+        <v>48.39</v>
+      </c>
+      <c r="D35">
+        <v>270</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>153.91999999999999</v>
+      </c>
+      <c r="C36">
+        <v>37.47</v>
+      </c>
+      <c r="D36">
+        <v>90</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>153.16</v>
+      </c>
+      <c r="C37">
+        <v>24</v>
+      </c>
+      <c r="D37">
+        <v>270</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>162.05000000000001</v>
+      </c>
+      <c r="C38">
+        <v>62.48</v>
+      </c>
+      <c r="D38">
+        <v>180</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>161.93</v>
+      </c>
+      <c r="C39">
+        <v>86.87</v>
+      </c>
+      <c r="D39">
+        <v>180</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40">
+        <v>162.05000000000001</v>
+      </c>
+      <c r="C40">
+        <v>61.21</v>
+      </c>
+      <c r="D40">
+        <v>180</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41">
+        <v>161.93</v>
+      </c>
+      <c r="C41">
+        <v>85.6</v>
+      </c>
+      <c r="D41">
+        <v>180</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>162.05000000000001</v>
+      </c>
+      <c r="C42">
+        <v>49.02</v>
+      </c>
+      <c r="D42">
+        <v>180</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>161.93</v>
+      </c>
+      <c r="C43">
+        <v>73.41</v>
+      </c>
+      <c r="D43">
+        <v>180</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G43" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>162.05000000000001</v>
+      </c>
+      <c r="C44">
+        <v>47.75</v>
+      </c>
+      <c r="D44">
+        <v>180</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45">
+        <v>161.93</v>
+      </c>
+      <c r="C45">
+        <v>72.14</v>
+      </c>
+      <c r="D45">
+        <v>180</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>2</v>
+      </c>
+      <c r="G45" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46">
+        <v>170.05</v>
+      </c>
+      <c r="C46">
+        <v>86.23</v>
+      </c>
+      <c r="D46">
+        <v>90</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47">
+        <v>169.29</v>
+      </c>
+      <c r="C47">
+        <v>72.77</v>
+      </c>
+      <c r="D47">
+        <v>270</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48">
+        <v>170.18</v>
+      </c>
+      <c r="C48">
+        <v>61.85</v>
+      </c>
+      <c r="D48">
+        <v>90</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <v>169.42</v>
+      </c>
+      <c r="C49">
+        <v>48.39</v>
+      </c>
+      <c r="D49">
+        <v>270</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50">
+        <v>108.33</v>
+      </c>
+      <c r="C50">
+        <v>29.97</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>150</v>
+      </c>
+      <c r="F50" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51">
+        <v>119.13</v>
+      </c>
+      <c r="C51">
+        <v>26.8</v>
+      </c>
+      <c r="D51">
+        <v>270</v>
+      </c>
+      <c r="E51" t="s">
+        <v>150</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52">
+        <v>108.33</v>
+      </c>
+      <c r="C52">
+        <v>28.19</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>153</v>
+      </c>
+      <c r="B53">
+        <v>120.78</v>
+      </c>
+      <c r="C53">
+        <v>27.05</v>
+      </c>
+      <c r="D53">
+        <v>270</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54">
+        <v>108.33</v>
+      </c>
+      <c r="C54">
+        <v>26.92</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>155</v>
+      </c>
+      <c r="F54" t="s">
+        <v>2</v>
+      </c>
+      <c r="G54" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55">
+        <v>121.92</v>
+      </c>
+      <c r="C55">
+        <v>27.05</v>
+      </c>
+      <c r="D55">
+        <v>270</v>
+      </c>
+      <c r="E55" t="s">
+        <v>155</v>
+      </c>
+      <c r="F55" t="s">
+        <v>2</v>
+      </c>
+      <c r="G55" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>211</v>
+      </c>
+      <c r="B56">
+        <v>59.69</v>
+      </c>
+      <c r="C56">
+        <v>22.99</v>
+      </c>
+      <c r="D56">
+        <v>180</v>
+      </c>
+      <c r="E56" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>2</v>
+      </c>
+      <c r="G56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>212</v>
+      </c>
+      <c r="B57">
+        <v>59.82</v>
+      </c>
+      <c r="C57">
+        <v>30.35</v>
+      </c>
+      <c r="D57">
+        <v>180</v>
+      </c>
+      <c r="E57" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>2</v>
+      </c>
+      <c r="G57" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>213</v>
+      </c>
+      <c r="B58">
+        <v>79.63</v>
+      </c>
+      <c r="C58">
+        <v>28.83</v>
+      </c>
+      <c r="D58">
+        <v>270</v>
+      </c>
+      <c r="E58" t="s">
+        <v>214</v>
+      </c>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>215</v>
+      </c>
+      <c r="B59">
+        <v>113.79</v>
+      </c>
+      <c r="C59">
+        <v>20.190000000000001</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>214</v>
+      </c>
+      <c r="F59" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>216</v>
+      </c>
+      <c r="B60">
+        <v>116.97</v>
+      </c>
+      <c r="C60">
+        <v>26.8</v>
+      </c>
+      <c r="D60">
+        <v>270</v>
+      </c>
+      <c r="E60" t="s">
+        <v>214</v>
+      </c>
+      <c r="F60" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61">
+        <v>75.819999999999993</v>
+      </c>
+      <c r="C61">
+        <v>27.94</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>53</v>
+      </c>
+      <c r="F61" t="s">
+        <v>54</v>
+      </c>
+      <c r="G61" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62">
+        <v>91.69</v>
+      </c>
+      <c r="C62">
+        <v>21.72</v>
+      </c>
+      <c r="D62">
+        <v>270</v>
+      </c>
+      <c r="E62" t="s">
+        <v>57</v>
+      </c>
+      <c r="F62" t="s">
+        <v>58</v>
+      </c>
+      <c r="G62" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>93.6</v>
+      </c>
+      <c r="C63">
+        <v>21.72</v>
+      </c>
+      <c r="D63">
+        <v>270</v>
+      </c>
+      <c r="E63" t="s">
+        <v>57</v>
+      </c>
+      <c r="F63" t="s">
+        <v>58</v>
+      </c>
+      <c r="G63" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>217</v>
+      </c>
+      <c r="B64">
+        <v>81.66</v>
+      </c>
+      <c r="C64">
+        <v>20.96</v>
+      </c>
+      <c r="D64">
+        <v>270</v>
+      </c>
+      <c r="E64" t="s">
+        <v>218</v>
+      </c>
+      <c r="F64" t="s">
+        <v>58</v>
+      </c>
+      <c r="G64" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>219</v>
+      </c>
+      <c r="B65">
+        <v>83.95</v>
+      </c>
+      <c r="C65">
+        <v>20.96</v>
+      </c>
+      <c r="D65">
+        <v>90</v>
+      </c>
+      <c r="E65" t="s">
+        <v>220</v>
+      </c>
+      <c r="F65" t="s">
+        <v>58</v>
+      </c>
+      <c r="G65" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66">
+        <v>137.16</v>
+      </c>
+      <c r="C66">
+        <v>82.17</v>
+      </c>
+      <c r="D66">
+        <v>90</v>
+      </c>
+      <c r="E66" t="s">
+        <v>61</v>
+      </c>
+      <c r="F66" t="s">
+        <v>62</v>
+      </c>
+      <c r="G66" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <v>137.29</v>
+      </c>
+      <c r="C67">
+        <v>57.79</v>
+      </c>
+      <c r="D67">
+        <v>90</v>
+      </c>
+      <c r="E67" t="s">
+        <v>61</v>
+      </c>
+      <c r="F67" t="s">
+        <v>62</v>
+      </c>
+      <c r="G67" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <v>137.29</v>
+      </c>
+      <c r="C68">
+        <v>33.4</v>
+      </c>
+      <c r="D68">
+        <v>90</v>
+      </c>
+      <c r="E68" t="s">
+        <v>61</v>
+      </c>
+      <c r="F68" t="s">
+        <v>62</v>
+      </c>
+      <c r="G68" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69">
+        <v>153.41999999999999</v>
+      </c>
+      <c r="C69">
+        <v>82.17</v>
+      </c>
+      <c r="D69">
+        <v>90</v>
+      </c>
+      <c r="E69" t="s">
+        <v>61</v>
+      </c>
+      <c r="F69" t="s">
+        <v>62</v>
+      </c>
+      <c r="G69" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70">
+        <v>153.54</v>
+      </c>
+      <c r="C70">
+        <v>57.66</v>
+      </c>
+      <c r="D70">
+        <v>90</v>
+      </c>
+      <c r="E70" t="s">
+        <v>61</v>
+      </c>
+      <c r="F70" t="s">
+        <v>62</v>
+      </c>
+      <c r="G70" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71">
+        <v>153.54</v>
+      </c>
+      <c r="C71">
+        <v>33.270000000000003</v>
+      </c>
+      <c r="D71">
+        <v>90</v>
+      </c>
+      <c r="E71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F71" t="s">
+        <v>62</v>
+      </c>
+      <c r="G71" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72">
+        <v>169.67</v>
+      </c>
+      <c r="C72">
+        <v>82.04</v>
+      </c>
+      <c r="D72">
+        <v>90</v>
+      </c>
+      <c r="E72" t="s">
+        <v>61</v>
+      </c>
+      <c r="F72" t="s">
+        <v>62</v>
+      </c>
+      <c r="G72" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73">
+        <v>169.8</v>
+      </c>
+      <c r="C73">
+        <v>57.66</v>
+      </c>
+      <c r="D73">
+        <v>90</v>
+      </c>
+      <c r="E73" t="s">
+        <v>61</v>
+      </c>
+      <c r="F73" t="s">
+        <v>62</v>
+      </c>
+      <c r="G73" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74">
+        <v>137.16</v>
+      </c>
+      <c r="C74">
+        <v>76.58</v>
+      </c>
+      <c r="D74">
+        <v>270</v>
+      </c>
+      <c r="E74" t="s">
+        <v>61</v>
+      </c>
+      <c r="F74" t="s">
+        <v>62</v>
+      </c>
+      <c r="G74" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>71</v>
+      </c>
+      <c r="B75">
+        <v>137.29</v>
+      </c>
+      <c r="C75">
+        <v>52.2</v>
+      </c>
+      <c r="D75">
+        <v>270</v>
+      </c>
+      <c r="E75" t="s">
+        <v>61</v>
+      </c>
+      <c r="F75" t="s">
+        <v>62</v>
+      </c>
+      <c r="G75" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B76">
+        <v>137.29</v>
+      </c>
+      <c r="C76">
+        <v>27.94</v>
+      </c>
+      <c r="D76">
+        <v>270</v>
+      </c>
+      <c r="E76" t="s">
+        <v>61</v>
+      </c>
+      <c r="F76" t="s">
+        <v>62</v>
+      </c>
+      <c r="G76" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>73</v>
+      </c>
+      <c r="B77">
+        <v>153.41999999999999</v>
+      </c>
+      <c r="C77">
+        <v>76.709999999999994</v>
+      </c>
+      <c r="D77">
+        <v>270</v>
+      </c>
+      <c r="E77" t="s">
+        <v>61</v>
+      </c>
+      <c r="F77" t="s">
+        <v>62</v>
+      </c>
+      <c r="G77" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>74</v>
+      </c>
+      <c r="B78">
+        <v>153.54</v>
+      </c>
+      <c r="C78">
+        <v>52.2</v>
+      </c>
+      <c r="D78">
+        <v>270</v>
+      </c>
+      <c r="E78" t="s">
+        <v>61</v>
+      </c>
+      <c r="F78" t="s">
+        <v>62</v>
+      </c>
+      <c r="G78" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>75</v>
+      </c>
+      <c r="B79">
+        <v>153.66999999999999</v>
+      </c>
+      <c r="C79">
+        <v>27.81</v>
+      </c>
+      <c r="D79">
+        <v>270</v>
+      </c>
+      <c r="E79" t="s">
+        <v>61</v>
+      </c>
+      <c r="F79" t="s">
+        <v>62</v>
+      </c>
+      <c r="G79" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>76</v>
+      </c>
+      <c r="B80">
+        <v>169.67</v>
+      </c>
+      <c r="C80">
+        <v>76.58</v>
+      </c>
+      <c r="D80">
+        <v>270</v>
+      </c>
+      <c r="E80" t="s">
+        <v>61</v>
+      </c>
+      <c r="F80" t="s">
+        <v>62</v>
+      </c>
+      <c r="G80" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81">
+        <v>169.8</v>
+      </c>
+      <c r="C81">
+        <v>52.2</v>
+      </c>
+      <c r="D81">
+        <v>270</v>
+      </c>
+      <c r="E81" t="s">
+        <v>61</v>
+      </c>
+      <c r="F81" t="s">
+        <v>62</v>
+      </c>
+      <c r="G81" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>78</v>
+      </c>
+      <c r="B82">
+        <v>139.94999999999999</v>
+      </c>
+      <c r="C82">
+        <v>86.23</v>
+      </c>
+      <c r="D82">
+        <v>90</v>
+      </c>
+      <c r="E82" t="s">
+        <v>79</v>
+      </c>
+      <c r="F82" t="s">
+        <v>80</v>
+      </c>
+      <c r="G82" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>139.32</v>
+      </c>
+      <c r="C83">
+        <v>72.77</v>
+      </c>
+      <c r="D83">
+        <v>270</v>
+      </c>
+      <c r="E83" t="s">
+        <v>79</v>
+      </c>
+      <c r="F83" t="s">
+        <v>80</v>
+      </c>
+      <c r="G83" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>140.08000000000001</v>
+      </c>
+      <c r="C84">
+        <v>61.85</v>
+      </c>
+      <c r="D84">
+        <v>90</v>
+      </c>
+      <c r="E84" t="s">
+        <v>79</v>
+      </c>
+      <c r="F84" t="s">
+        <v>80</v>
+      </c>
+      <c r="G84" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>139.44999999999999</v>
+      </c>
+      <c r="C85">
+        <v>48.39</v>
+      </c>
+      <c r="D85">
+        <v>270</v>
+      </c>
+      <c r="E85" t="s">
+        <v>79</v>
+      </c>
+      <c r="F85" t="s">
+        <v>80</v>
+      </c>
+      <c r="G85" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>140.08000000000001</v>
+      </c>
+      <c r="C86">
+        <v>37.47</v>
+      </c>
+      <c r="D86">
+        <v>90</v>
+      </c>
+      <c r="E86" t="s">
+        <v>79</v>
+      </c>
+      <c r="F86" t="s">
+        <v>80</v>
+      </c>
+      <c r="G86" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>139.44999999999999</v>
+      </c>
+      <c r="C87">
+        <v>24</v>
+      </c>
+      <c r="D87">
+        <v>270</v>
+      </c>
+      <c r="E87" t="s">
+        <v>79</v>
+      </c>
+      <c r="F87" t="s">
+        <v>80</v>
+      </c>
+      <c r="G87" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>156.21</v>
+      </c>
+      <c r="C88">
+        <v>86.23</v>
+      </c>
+      <c r="D88">
+        <v>90</v>
+      </c>
+      <c r="E88" t="s">
+        <v>79</v>
+      </c>
+      <c r="F88" t="s">
+        <v>80</v>
+      </c>
+      <c r="G88" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>155.58000000000001</v>
+      </c>
+      <c r="C89">
+        <v>72.77</v>
+      </c>
+      <c r="D89">
+        <v>270</v>
+      </c>
+      <c r="E89" t="s">
+        <v>79</v>
+      </c>
+      <c r="F89" t="s">
+        <v>80</v>
+      </c>
+      <c r="G89" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>156.34</v>
+      </c>
+      <c r="C90">
+        <v>61.85</v>
+      </c>
+      <c r="D90">
+        <v>90</v>
+      </c>
+      <c r="E90" t="s">
+        <v>79</v>
+      </c>
+      <c r="F90" t="s">
+        <v>80</v>
+      </c>
+      <c r="G90" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>155.69999999999999</v>
+      </c>
+      <c r="C91">
+        <v>48.39</v>
+      </c>
+      <c r="D91">
+        <v>270</v>
+      </c>
+      <c r="E91" t="s">
+        <v>79</v>
+      </c>
+      <c r="F91" t="s">
+        <v>80</v>
+      </c>
+      <c r="G91" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>156.34</v>
+      </c>
+      <c r="C92">
+        <v>37.47</v>
+      </c>
+      <c r="D92">
+        <v>90</v>
+      </c>
+      <c r="E92" t="s">
+        <v>79</v>
+      </c>
+      <c r="F92" t="s">
+        <v>80</v>
+      </c>
+      <c r="G92" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>155.69999999999999</v>
+      </c>
+      <c r="C93">
+        <v>24</v>
+      </c>
+      <c r="D93">
+        <v>270</v>
+      </c>
+      <c r="E93" t="s">
+        <v>79</v>
+      </c>
+      <c r="F93" t="s">
+        <v>80</v>
+      </c>
+      <c r="G93" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>172.47</v>
+      </c>
+      <c r="C94">
+        <v>86.23</v>
+      </c>
+      <c r="D94">
+        <v>90</v>
+      </c>
+      <c r="E94" t="s">
+        <v>79</v>
+      </c>
+      <c r="F94" t="s">
+        <v>80</v>
+      </c>
+      <c r="G94" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>171.83</v>
+      </c>
+      <c r="C95">
+        <v>72.77</v>
+      </c>
+      <c r="D95">
+        <v>270</v>
+      </c>
+      <c r="E95" t="s">
+        <v>79</v>
+      </c>
+      <c r="F95" t="s">
+        <v>80</v>
+      </c>
+      <c r="G95" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>172.59</v>
+      </c>
+      <c r="C96">
+        <v>61.85</v>
+      </c>
+      <c r="D96">
+        <v>90</v>
+      </c>
+      <c r="E96" t="s">
+        <v>79</v>
+      </c>
+      <c r="F96" t="s">
+        <v>80</v>
+      </c>
+      <c r="G96" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>171.96</v>
+      </c>
+      <c r="C97">
+        <v>48.39</v>
+      </c>
+      <c r="D97">
+        <v>270</v>
+      </c>
+      <c r="E97" t="s">
+        <v>79</v>
+      </c>
+      <c r="F97" t="s">
+        <v>80</v>
+      </c>
+      <c r="G97" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>90.3</v>
+      </c>
+      <c r="C98">
+        <v>21.97</v>
+      </c>
+      <c r="D98">
+        <v>90</v>
+      </c>
+      <c r="E98" t="s">
+        <v>97</v>
+      </c>
+      <c r="F98" t="s">
+        <v>62</v>
+      </c>
+      <c r="G98" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>95</v>
+      </c>
+      <c r="C99">
+        <v>21.59</v>
+      </c>
+      <c r="D99">
+        <v>90</v>
+      </c>
+      <c r="E99" t="s">
+        <v>97</v>
+      </c>
+      <c r="F99" t="s">
+        <v>62</v>
+      </c>
+      <c r="G99" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>221</v>
+      </c>
+      <c r="B100">
+        <v>82.55</v>
+      </c>
+      <c r="C100">
+        <v>25.27</v>
+      </c>
+      <c r="D100">
+        <v>180</v>
+      </c>
+      <c r="E100" t="s">
+        <v>222</v>
+      </c>
+      <c r="F100" t="s">
+        <v>62</v>
+      </c>
+      <c r="G100" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>223</v>
+      </c>
+      <c r="B101">
+        <v>87.5</v>
+      </c>
+      <c r="C101">
+        <v>21.34</v>
+      </c>
+      <c r="D101">
+        <v>90</v>
+      </c>
+      <c r="E101">
+        <v>470</v>
+      </c>
+      <c r="F101" t="s">
+        <v>62</v>
+      </c>
+      <c r="G101" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>224</v>
+      </c>
+      <c r="B102">
+        <v>86.36</v>
+      </c>
+      <c r="C102">
+        <v>21.34</v>
+      </c>
+      <c r="D102">
+        <v>90</v>
+      </c>
+      <c r="E102" t="s">
+        <v>97</v>
+      </c>
+      <c r="F102" t="s">
+        <v>62</v>
+      </c>
+      <c r="G102" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>99</v>
+      </c>
+      <c r="B103">
+        <v>133.86000000000001</v>
+      </c>
+      <c r="C103">
+        <v>61.85</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103" t="s">
+        <v>100</v>
+      </c>
+      <c r="F103" t="s">
+        <v>101</v>
+      </c>
+      <c r="G103" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>133.86000000000001</v>
+      </c>
+      <c r="C104">
+        <v>37.47</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104" t="s">
+        <v>100</v>
+      </c>
+      <c r="F104" t="s">
+        <v>101</v>
+      </c>
+      <c r="G104" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>133.72999999999999</v>
+      </c>
+      <c r="C105">
+        <v>86.23</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105" t="s">
+        <v>100</v>
+      </c>
+      <c r="F105" t="s">
+        <v>101</v>
+      </c>
+      <c r="G105" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>133.86000000000001</v>
+      </c>
+      <c r="C106">
+        <v>48.26</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106" t="s">
+        <v>100</v>
+      </c>
+      <c r="F106" t="s">
+        <v>101</v>
+      </c>
+      <c r="G106" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <v>133.86000000000001</v>
+      </c>
+      <c r="C107">
+        <v>23.88</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107" t="s">
+        <v>100</v>
+      </c>
+      <c r="F107" t="s">
+        <v>101</v>
+      </c>
+      <c r="G107" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <v>133.72999999999999</v>
+      </c>
+      <c r="C108">
+        <v>72.64</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108" t="s">
+        <v>100</v>
+      </c>
+      <c r="F108" t="s">
+        <v>101</v>
+      </c>
+      <c r="G108" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <v>150.11000000000001</v>
+      </c>
+      <c r="C109">
+        <v>61.85</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109" t="s">
+        <v>100</v>
+      </c>
+      <c r="F109" t="s">
+        <v>101</v>
+      </c>
+      <c r="G109" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>150.11000000000001</v>
+      </c>
+      <c r="C110">
+        <v>37.47</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110" t="s">
+        <v>100</v>
+      </c>
+      <c r="F110" t="s">
+        <v>101</v>
+      </c>
+      <c r="G110" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>149.99</v>
+      </c>
+      <c r="C111">
+        <v>86.23</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111" t="s">
+        <v>100</v>
+      </c>
+      <c r="F111" t="s">
+        <v>101</v>
+      </c>
+      <c r="G111" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <v>150.11000000000001</v>
+      </c>
+      <c r="C112">
+        <v>48.26</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112" t="s">
+        <v>100</v>
+      </c>
+      <c r="F112" t="s">
+        <v>101</v>
+      </c>
+      <c r="G112" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>150.11000000000001</v>
+      </c>
+      <c r="C113">
+        <v>23.88</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113" t="s">
+        <v>100</v>
+      </c>
+      <c r="F113" t="s">
+        <v>101</v>
+      </c>
+      <c r="G113" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <v>149.99</v>
+      </c>
+      <c r="C114">
+        <v>72.64</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114" t="s">
+        <v>100</v>
+      </c>
+      <c r="F114" t="s">
+        <v>101</v>
+      </c>
+      <c r="G114" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>113</v>
+      </c>
+      <c r="B115">
+        <v>166.37</v>
+      </c>
+      <c r="C115">
+        <v>61.85</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115" t="s">
+        <v>100</v>
+      </c>
+      <c r="F115" t="s">
+        <v>101</v>
+      </c>
+      <c r="G115" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <v>166.24</v>
+      </c>
+      <c r="C116">
+        <v>86.23</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116" t="s">
+        <v>100</v>
+      </c>
+      <c r="F116" t="s">
+        <v>101</v>
+      </c>
+      <c r="G116" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <v>166.37</v>
+      </c>
+      <c r="C117">
+        <v>48.26</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117" t="s">
+        <v>100</v>
+      </c>
+      <c r="F117" t="s">
+        <v>101</v>
+      </c>
+      <c r="G117" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <v>166.24</v>
+      </c>
+      <c r="C118">
+        <v>72.64</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118" t="s">
+        <v>100</v>
+      </c>
+      <c r="F118" t="s">
+        <v>101</v>
+      </c>
+      <c r="G118" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>225</v>
+      </c>
+      <c r="B119">
+        <v>60.33</v>
+      </c>
+      <c r="C119">
+        <v>26.54</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119" t="s">
+        <v>100</v>
+      </c>
+      <c r="F119" t="s">
+        <v>101</v>
+      </c>
+      <c r="G119" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>226</v>
+      </c>
+      <c r="B120">
+        <v>82.8</v>
+      </c>
+      <c r="C120">
+        <v>28.83</v>
+      </c>
+      <c r="D120">
+        <v>90</v>
+      </c>
+      <c r="E120" t="s">
+        <v>227</v>
+      </c>
+      <c r="F120" t="s">
+        <v>228</v>
+      </c>
+      <c r="G120" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>229</v>
+      </c>
+      <c r="B121">
+        <v>113.16</v>
+      </c>
+      <c r="C121">
+        <v>25.27</v>
+      </c>
+      <c r="D121">
+        <v>90</v>
+      </c>
+      <c r="E121" t="s">
+        <v>230</v>
+      </c>
+      <c r="F121" t="s">
+        <v>231</v>
+      </c>
+      <c r="G121" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>232</v>
+      </c>
+      <c r="B122">
+        <v>75.69</v>
+      </c>
+      <c r="C122">
+        <v>21.53</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122" t="s">
+        <v>233</v>
+      </c>
+      <c r="G122" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>117</v>
+      </c>
+      <c r="B123">
+        <v>129.54</v>
+      </c>
+      <c r="C123">
+        <v>54.23</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123" t="s">
+        <v>1</v>
+      </c>
+      <c r="F123" t="s">
+        <v>2</v>
+      </c>
+      <c r="G123" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>118</v>
+      </c>
+      <c r="B124">
+        <v>129.54</v>
+      </c>
+      <c r="C124">
+        <v>29.85</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124" t="s">
+        <v>1</v>
+      </c>
+      <c r="F124" t="s">
+        <v>2</v>
+      </c>
+      <c r="G124" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>119</v>
+      </c>
+      <c r="B125">
+        <v>129.41</v>
+      </c>
+      <c r="C125">
+        <v>78.61</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125" t="s">
+        <v>1</v>
+      </c>
+      <c r="F125" t="s">
+        <v>2</v>
+      </c>
+      <c r="G125" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>120</v>
+      </c>
+      <c r="B126">
+        <v>129.54</v>
+      </c>
+      <c r="C126">
+        <v>55.5</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126" t="s">
+        <v>1</v>
+      </c>
+      <c r="F126" t="s">
+        <v>2</v>
+      </c>
+      <c r="G126" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>121</v>
+      </c>
+      <c r="B127">
+        <v>129.54</v>
+      </c>
+      <c r="C127">
+        <v>31.12</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127" t="s">
+        <v>1</v>
+      </c>
+      <c r="F127" t="s">
+        <v>2</v>
+      </c>
+      <c r="G127" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>122</v>
+      </c>
+      <c r="B128">
+        <v>129.41</v>
+      </c>
+      <c r="C128">
+        <v>80.010000000000005</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128" t="s">
+        <v>1</v>
+      </c>
+      <c r="F128" t="s">
+        <v>2</v>
+      </c>
+      <c r="G128" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>123</v>
+      </c>
+      <c r="B129">
+        <v>137.54</v>
+      </c>
+      <c r="C129">
+        <v>86.23</v>
+      </c>
+      <c r="D129">
+        <v>90</v>
+      </c>
+      <c r="E129" t="s">
+        <v>15</v>
+      </c>
+      <c r="F129" t="s">
+        <v>16</v>
+      </c>
+      <c r="G129" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>124</v>
+      </c>
+      <c r="B130">
+        <v>136.78</v>
+      </c>
+      <c r="C130">
+        <v>72.77</v>
+      </c>
+      <c r="D130">
+        <v>270</v>
+      </c>
+      <c r="E130" t="s">
+        <v>15</v>
+      </c>
+      <c r="F130" t="s">
+        <v>16</v>
+      </c>
+      <c r="G130" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>125</v>
+      </c>
+      <c r="B131">
+        <v>137.66999999999999</v>
+      </c>
+      <c r="C131">
+        <v>61.85</v>
+      </c>
+      <c r="D131">
+        <v>90</v>
+      </c>
+      <c r="E131" t="s">
+        <v>15</v>
+      </c>
+      <c r="F131" t="s">
+        <v>16</v>
+      </c>
+      <c r="G131" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>126</v>
+      </c>
+      <c r="B132">
+        <v>136.91</v>
+      </c>
+      <c r="C132">
+        <v>48.39</v>
+      </c>
+      <c r="D132">
+        <v>270</v>
+      </c>
+      <c r="E132" t="s">
+        <v>15</v>
+      </c>
+      <c r="F132" t="s">
+        <v>16</v>
+      </c>
+      <c r="G132" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>127</v>
+      </c>
+      <c r="B133">
+        <v>137.66999999999999</v>
+      </c>
+      <c r="C133">
+        <v>37.47</v>
+      </c>
+      <c r="D133">
+        <v>90</v>
+      </c>
+      <c r="E133" t="s">
+        <v>15</v>
+      </c>
+      <c r="F133" t="s">
+        <v>16</v>
+      </c>
+      <c r="G133" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>128</v>
+      </c>
+      <c r="B134">
+        <v>136.91</v>
+      </c>
+      <c r="C134">
+        <v>24</v>
+      </c>
+      <c r="D134">
+        <v>270</v>
+      </c>
+      <c r="E134" t="s">
+        <v>15</v>
+      </c>
+      <c r="F134" t="s">
+        <v>16</v>
+      </c>
+      <c r="G134" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>129</v>
+      </c>
+      <c r="B135">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C135">
+        <v>54.36</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135" t="s">
+        <v>1</v>
+      </c>
+      <c r="F135" t="s">
+        <v>2</v>
+      </c>
+      <c r="G135" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>130</v>
+      </c>
+      <c r="B136">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C136">
+        <v>29.85</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136" t="s">
+        <v>1</v>
+      </c>
+      <c r="F136" t="s">
+        <v>2</v>
+      </c>
+      <c r="G136" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>131</v>
+      </c>
+      <c r="B137">
+        <v>145.66999999999999</v>
+      </c>
+      <c r="C137">
+        <v>78.61</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137" t="s">
+        <v>1</v>
+      </c>
+      <c r="F137" t="s">
+        <v>2</v>
+      </c>
+      <c r="G137" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>132</v>
+      </c>
+      <c r="B138">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C138">
+        <v>55.63</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138" t="s">
+        <v>1</v>
+      </c>
+      <c r="F138" t="s">
+        <v>2</v>
+      </c>
+      <c r="G138" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>133</v>
+      </c>
+      <c r="B139">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="C139">
+        <v>31.12</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139" t="s">
+        <v>1</v>
+      </c>
+      <c r="F139" t="s">
+        <v>2</v>
+      </c>
+      <c r="G139" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>134</v>
+      </c>
+      <c r="B140">
+        <v>145.66999999999999</v>
+      </c>
+      <c r="C140">
+        <v>79.88</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140" t="s">
+        <v>1</v>
+      </c>
+      <c r="F140" t="s">
+        <v>2</v>
+      </c>
+      <c r="G140" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>135</v>
+      </c>
+      <c r="B141">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="C141">
+        <v>86.23</v>
+      </c>
+      <c r="D141">
+        <v>90</v>
+      </c>
+      <c r="E141" t="s">
+        <v>15</v>
+      </c>
+      <c r="F141" t="s">
+        <v>16</v>
+      </c>
+      <c r="G141" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>136</v>
+      </c>
+      <c r="B142">
+        <v>153.03</v>
+      </c>
+      <c r="C142">
+        <v>72.77</v>
+      </c>
+      <c r="D142">
+        <v>270</v>
+      </c>
+      <c r="E142" t="s">
+        <v>15</v>
+      </c>
+      <c r="F142" t="s">
+        <v>16</v>
+      </c>
+      <c r="G142" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>137</v>
+      </c>
+      <c r="B143">
+        <v>153.91999999999999</v>
+      </c>
+      <c r="C143">
+        <v>61.85</v>
+      </c>
+      <c r="D143">
+        <v>90</v>
+      </c>
+      <c r="E143" t="s">
+        <v>15</v>
+      </c>
+      <c r="F143" t="s">
+        <v>16</v>
+      </c>
+      <c r="G143" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>138</v>
+      </c>
+      <c r="B144">
+        <v>153.16</v>
+      </c>
+      <c r="C144">
+        <v>48.39</v>
+      </c>
+      <c r="D144">
+        <v>270</v>
+      </c>
+      <c r="E144" t="s">
+        <v>15</v>
+      </c>
+      <c r="F144" t="s">
+        <v>16</v>
+      </c>
+      <c r="G144" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>139</v>
+      </c>
+      <c r="B145">
+        <v>153.91999999999999</v>
+      </c>
+      <c r="C145">
+        <v>37.47</v>
+      </c>
+      <c r="D145">
+        <v>90</v>
+      </c>
+      <c r="E145" t="s">
+        <v>15</v>
+      </c>
+      <c r="F145" t="s">
+        <v>16</v>
+      </c>
+      <c r="G145" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>140</v>
+      </c>
+      <c r="B146">
+        <v>153.16</v>
+      </c>
+      <c r="C146">
+        <v>24</v>
+      </c>
+      <c r="D146">
+        <v>270</v>
+      </c>
+      <c r="E146" t="s">
+        <v>15</v>
+      </c>
+      <c r="F146" t="s">
+        <v>16</v>
+      </c>
+      <c r="G146" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>141</v>
+      </c>
+      <c r="B147">
+        <v>162.05000000000001</v>
+      </c>
+      <c r="C147">
+        <v>54.36</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147" t="s">
+        <v>1</v>
+      </c>
+      <c r="F147" t="s">
+        <v>2</v>
+      </c>
+      <c r="G147" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>142</v>
+      </c>
+      <c r="B148">
+        <v>161.93</v>
+      </c>
+      <c r="C148">
+        <v>78.739999999999995</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
+      <c r="E148" t="s">
+        <v>1</v>
+      </c>
+      <c r="F148" t="s">
+        <v>2</v>
+      </c>
+      <c r="G148" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>143</v>
+      </c>
+      <c r="B149">
+        <v>162.05000000000001</v>
+      </c>
+      <c r="C149">
+        <v>55.63</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149" t="s">
+        <v>1</v>
+      </c>
+      <c r="F149" t="s">
+        <v>2</v>
+      </c>
+      <c r="G149" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>144</v>
+      </c>
+      <c r="B150">
+        <v>161.93</v>
+      </c>
+      <c r="C150">
+        <v>80.010000000000005</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150" t="s">
+        <v>1</v>
+      </c>
+      <c r="F150" t="s">
+        <v>2</v>
+      </c>
+      <c r="G150" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>145</v>
+      </c>
+      <c r="B151">
+        <v>170.05</v>
+      </c>
+      <c r="C151">
+        <v>86.23</v>
+      </c>
+      <c r="D151">
+        <v>90</v>
+      </c>
+      <c r="E151" t="s">
+        <v>15</v>
+      </c>
+      <c r="F151" t="s">
+        <v>16</v>
+      </c>
+      <c r="G151" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>146</v>
+      </c>
+      <c r="B152">
+        <v>169.29</v>
+      </c>
+      <c r="C152">
+        <v>72.77</v>
+      </c>
+      <c r="D152">
+        <v>270</v>
+      </c>
+      <c r="E152" t="s">
+        <v>15</v>
+      </c>
+      <c r="F152" t="s">
+        <v>16</v>
+      </c>
+      <c r="G152" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>147</v>
+      </c>
+      <c r="B153">
+        <v>170.18</v>
+      </c>
+      <c r="C153">
+        <v>61.85</v>
+      </c>
+      <c r="D153">
+        <v>90</v>
+      </c>
+      <c r="E153" t="s">
+        <v>15</v>
+      </c>
+      <c r="F153" t="s">
+        <v>16</v>
+      </c>
+      <c r="G153" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>148</v>
+      </c>
+      <c r="B154">
+        <v>169.42</v>
+      </c>
+      <c r="C154">
+        <v>48.39</v>
+      </c>
+      <c r="D154">
+        <v>270</v>
+      </c>
+      <c r="E154" t="s">
+        <v>15</v>
+      </c>
+      <c r="F154" t="s">
+        <v>16</v>
+      </c>
+      <c r="G154" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>234</v>
+      </c>
+      <c r="B155">
+        <v>59.69</v>
+      </c>
+      <c r="C155">
+        <v>22.99</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155" t="s">
+        <v>1</v>
+      </c>
+      <c r="F155" t="s">
+        <v>2</v>
+      </c>
+      <c r="G155" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>235</v>
+      </c>
+      <c r="B156">
+        <v>59.82</v>
+      </c>
+      <c r="C156">
+        <v>30.48</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156" t="s">
+        <v>1</v>
+      </c>
+      <c r="F156" t="s">
+        <v>2</v>
+      </c>
+      <c r="G156" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>55</v>
+      </c>
+      <c r="B157">
+        <v>88.27</v>
+      </c>
+      <c r="C157">
+        <v>27.69</v>
+      </c>
+      <c r="D157">
+        <v>90</v>
+      </c>
+      <c r="E157" t="s">
+        <v>53</v>
+      </c>
+      <c r="F157" t="s">
+        <v>54</v>
+      </c>
+      <c r="G157" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>162</v>
+      </c>
+      <c r="B158">
+        <v>130.30000000000001</v>
+      </c>
+      <c r="C158">
+        <v>82.3</v>
+      </c>
+      <c r="D158">
+        <v>90</v>
+      </c>
+      <c r="E158" t="s">
+        <v>61</v>
+      </c>
+      <c r="F158" t="s">
+        <v>62</v>
+      </c>
+      <c r="G158" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>163</v>
+      </c>
+      <c r="B159">
+        <v>130.18</v>
+      </c>
+      <c r="C159">
+        <v>57.79</v>
+      </c>
+      <c r="D159">
+        <v>90</v>
+      </c>
+      <c r="E159" t="s">
+        <v>61</v>
+      </c>
+      <c r="F159" t="s">
+        <v>62</v>
+      </c>
+      <c r="G159" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>164</v>
+      </c>
+      <c r="B160">
+        <v>130.18</v>
+      </c>
+      <c r="C160">
+        <v>33.270000000000003</v>
+      </c>
+      <c r="D160">
+        <v>90</v>
+      </c>
+      <c r="E160" t="s">
+        <v>61</v>
+      </c>
+      <c r="F160" t="s">
+        <v>62</v>
+      </c>
+      <c r="G160" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>165</v>
+      </c>
+      <c r="B161">
+        <v>146.56</v>
+      </c>
+      <c r="C161">
+        <v>82.17</v>
+      </c>
+      <c r="D161">
+        <v>90</v>
+      </c>
+      <c r="E161" t="s">
+        <v>61</v>
+      </c>
+      <c r="F161" t="s">
+        <v>62</v>
+      </c>
+      <c r="G161" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>166</v>
+      </c>
+      <c r="B162">
+        <v>146.69</v>
+      </c>
+      <c r="C162">
+        <v>57.79</v>
+      </c>
+      <c r="D162">
+        <v>90</v>
+      </c>
+      <c r="E162" t="s">
+        <v>61</v>
+      </c>
+      <c r="F162" t="s">
+        <v>62</v>
+      </c>
+      <c r="G162" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>167</v>
+      </c>
+      <c r="B163">
+        <v>146.69</v>
+      </c>
+      <c r="C163">
+        <v>33.4</v>
+      </c>
+      <c r="D163">
+        <v>90</v>
+      </c>
+      <c r="E163" t="s">
+        <v>61</v>
+      </c>
+      <c r="F163" t="s">
+        <v>62</v>
+      </c>
+      <c r="G163" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>168</v>
+      </c>
+      <c r="B164">
+        <v>162.81</v>
+      </c>
+      <c r="C164">
+        <v>82.17</v>
+      </c>
+      <c r="D164">
+        <v>90</v>
+      </c>
+      <c r="E164" t="s">
+        <v>61</v>
+      </c>
+      <c r="F164" t="s">
+        <v>62</v>
+      </c>
+      <c r="G164" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>169</v>
+      </c>
+      <c r="B165">
+        <v>162.94</v>
+      </c>
+      <c r="C165">
+        <v>57.79</v>
+      </c>
+      <c r="D165">
+        <v>90</v>
+      </c>
+      <c r="E165" t="s">
+        <v>61</v>
+      </c>
+      <c r="F165" t="s">
+        <v>62</v>
+      </c>
+      <c r="G165" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>170</v>
+      </c>
+      <c r="B166">
+        <v>130.30000000000001</v>
+      </c>
+      <c r="C166">
+        <v>76.45</v>
+      </c>
+      <c r="D166">
+        <v>270</v>
+      </c>
+      <c r="E166" t="s">
+        <v>61</v>
+      </c>
+      <c r="F166" t="s">
+        <v>62</v>
+      </c>
+      <c r="G166" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>171</v>
+      </c>
+      <c r="B167">
+        <v>129.91999999999999</v>
+      </c>
+      <c r="C167">
+        <v>52.07</v>
+      </c>
+      <c r="D167">
+        <v>270</v>
+      </c>
+      <c r="E167" t="s">
+        <v>61</v>
+      </c>
+      <c r="F167" t="s">
+        <v>62</v>
+      </c>
+      <c r="G167" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>172</v>
+      </c>
+      <c r="B168">
+        <v>130.18</v>
+      </c>
+      <c r="C168">
+        <v>27.69</v>
+      </c>
+      <c r="D168">
+        <v>270</v>
+      </c>
+      <c r="E168" t="s">
+        <v>61</v>
+      </c>
+      <c r="F168" t="s">
+        <v>62</v>
+      </c>
+      <c r="G168" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>173</v>
+      </c>
+      <c r="B169">
+        <v>146.56</v>
+      </c>
+      <c r="C169">
+        <v>76.45</v>
+      </c>
+      <c r="D169">
+        <v>270</v>
+      </c>
+      <c r="E169" t="s">
+        <v>61</v>
+      </c>
+      <c r="F169" t="s">
+        <v>62</v>
+      </c>
+      <c r="G169" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>174</v>
+      </c>
+      <c r="B170">
+        <v>146.69</v>
+      </c>
+      <c r="C170">
+        <v>52.07</v>
+      </c>
+      <c r="D170">
+        <v>270</v>
+      </c>
+      <c r="E170" t="s">
+        <v>61</v>
+      </c>
+      <c r="F170" t="s">
+        <v>62</v>
+      </c>
+      <c r="G170" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>175</v>
+      </c>
+      <c r="B171">
+        <v>146.69</v>
+      </c>
+      <c r="C171">
+        <v>27.69</v>
+      </c>
+      <c r="D171">
+        <v>270</v>
+      </c>
+      <c r="E171" t="s">
+        <v>61</v>
+      </c>
+      <c r="F171" t="s">
+        <v>62</v>
+      </c>
+      <c r="G171" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>176</v>
+      </c>
+      <c r="B172">
+        <v>162.81</v>
+      </c>
+      <c r="C172">
+        <v>76.58</v>
+      </c>
+      <c r="D172">
+        <v>270</v>
+      </c>
+      <c r="E172" t="s">
+        <v>61</v>
+      </c>
+      <c r="F172" t="s">
+        <v>62</v>
+      </c>
+      <c r="G172" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>177</v>
+      </c>
+      <c r="B173">
+        <v>162.94</v>
+      </c>
+      <c r="C173">
+        <v>52.07</v>
+      </c>
+      <c r="D173">
+        <v>270</v>
+      </c>
+      <c r="E173" t="s">
+        <v>61</v>
+      </c>
+      <c r="F173" t="s">
+        <v>62</v>
+      </c>
+      <c r="G173" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>178</v>
+      </c>
+      <c r="B174">
+        <v>139.94999999999999</v>
+      </c>
+      <c r="C174">
+        <v>86.23</v>
+      </c>
+      <c r="D174">
+        <v>90</v>
+      </c>
+      <c r="E174" t="s">
+        <v>79</v>
+      </c>
+      <c r="F174" t="s">
+        <v>80</v>
+      </c>
+      <c r="G174" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>179</v>
+      </c>
+      <c r="B175">
+        <v>139.32</v>
+      </c>
+      <c r="C175">
+        <v>72.77</v>
+      </c>
+      <c r="D175">
+        <v>270</v>
+      </c>
+      <c r="E175" t="s">
+        <v>79</v>
+      </c>
+      <c r="F175" t="s">
+        <v>80</v>
+      </c>
+      <c r="G175" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>180</v>
+      </c>
+      <c r="B176">
+        <v>140.08000000000001</v>
+      </c>
+      <c r="C176">
+        <v>61.85</v>
+      </c>
+      <c r="D176">
+        <v>90</v>
+      </c>
+      <c r="E176" t="s">
+        <v>79</v>
+      </c>
+      <c r="F176" t="s">
+        <v>80</v>
+      </c>
+      <c r="G176" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>181</v>
+      </c>
+      <c r="B177">
+        <v>139.44999999999999</v>
+      </c>
+      <c r="C177">
+        <v>48.39</v>
+      </c>
+      <c r="D177">
+        <v>270</v>
+      </c>
+      <c r="E177" t="s">
+        <v>79</v>
+      </c>
+      <c r="F177" t="s">
+        <v>80</v>
+      </c>
+      <c r="G177" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>182</v>
+      </c>
+      <c r="B178">
+        <v>140.08000000000001</v>
+      </c>
+      <c r="C178">
+        <v>37.47</v>
+      </c>
+      <c r="D178">
+        <v>90</v>
+      </c>
+      <c r="E178" t="s">
+        <v>79</v>
+      </c>
+      <c r="F178" t="s">
+        <v>80</v>
+      </c>
+      <c r="G178" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>183</v>
+      </c>
+      <c r="B179">
+        <v>139.44999999999999</v>
+      </c>
+      <c r="C179">
+        <v>24</v>
+      </c>
+      <c r="D179">
+        <v>270</v>
+      </c>
+      <c r="E179" t="s">
+        <v>79</v>
+      </c>
+      <c r="F179" t="s">
+        <v>80</v>
+      </c>
+      <c r="G179" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>184</v>
+      </c>
+      <c r="B180">
+        <v>156.21</v>
+      </c>
+      <c r="C180">
+        <v>86.23</v>
+      </c>
+      <c r="D180">
+        <v>90</v>
+      </c>
+      <c r="E180" t="s">
+        <v>79</v>
+      </c>
+      <c r="F180" t="s">
+        <v>80</v>
+      </c>
+      <c r="G180" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>185</v>
+      </c>
+      <c r="B181">
+        <v>155.58000000000001</v>
+      </c>
+      <c r="C181">
+        <v>72.77</v>
+      </c>
+      <c r="D181">
+        <v>270</v>
+      </c>
+      <c r="E181" t="s">
+        <v>79</v>
+      </c>
+      <c r="F181" t="s">
+        <v>80</v>
+      </c>
+      <c r="G181" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>186</v>
+      </c>
+      <c r="B182">
+        <v>156.34</v>
+      </c>
+      <c r="C182">
+        <v>61.85</v>
+      </c>
+      <c r="D182">
+        <v>90</v>
+      </c>
+      <c r="E182" t="s">
+        <v>79</v>
+      </c>
+      <c r="F182" t="s">
+        <v>80</v>
+      </c>
+      <c r="G182" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>187</v>
+      </c>
+      <c r="B183">
+        <v>155.69999999999999</v>
+      </c>
+      <c r="C183">
+        <v>48.39</v>
+      </c>
+      <c r="D183">
+        <v>270</v>
+      </c>
+      <c r="E183" t="s">
+        <v>79</v>
+      </c>
+      <c r="F183" t="s">
+        <v>80</v>
+      </c>
+      <c r="G183" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>188</v>
+      </c>
+      <c r="B184">
+        <v>156.34</v>
+      </c>
+      <c r="C184">
+        <v>37.47</v>
+      </c>
+      <c r="D184">
+        <v>90</v>
+      </c>
+      <c r="E184" t="s">
+        <v>79</v>
+      </c>
+      <c r="F184" t="s">
+        <v>80</v>
+      </c>
+      <c r="G184" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>189</v>
+      </c>
+      <c r="B185">
+        <v>155.69999999999999</v>
+      </c>
+      <c r="C185">
+        <v>24</v>
+      </c>
+      <c r="D185">
+        <v>270</v>
+      </c>
+      <c r="E185" t="s">
+        <v>79</v>
+      </c>
+      <c r="F185" t="s">
+        <v>80</v>
+      </c>
+      <c r="G185" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>190</v>
+      </c>
+      <c r="B186">
+        <v>172.47</v>
+      </c>
+      <c r="C186">
+        <v>86.23</v>
+      </c>
+      <c r="D186">
+        <v>90</v>
+      </c>
+      <c r="E186" t="s">
+        <v>79</v>
+      </c>
+      <c r="F186" t="s">
+        <v>80</v>
+      </c>
+      <c r="G186" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>191</v>
+      </c>
+      <c r="B187">
+        <v>171.83</v>
+      </c>
+      <c r="C187">
+        <v>72.77</v>
+      </c>
+      <c r="D187">
+        <v>270</v>
+      </c>
+      <c r="E187" t="s">
+        <v>79</v>
+      </c>
+      <c r="F187" t="s">
+        <v>80</v>
+      </c>
+      <c r="G187" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>192</v>
+      </c>
+      <c r="B188">
+        <v>172.59</v>
+      </c>
+      <c r="C188">
+        <v>61.85</v>
+      </c>
+      <c r="D188">
+        <v>90</v>
+      </c>
+      <c r="E188" t="s">
+        <v>79</v>
+      </c>
+      <c r="F188" t="s">
+        <v>80</v>
+      </c>
+      <c r="G188" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>193</v>
+      </c>
+      <c r="B189">
+        <v>171.96</v>
+      </c>
+      <c r="C189">
+        <v>48.39</v>
+      </c>
+      <c r="D189">
+        <v>270</v>
+      </c>
+      <c r="E189" t="s">
+        <v>79</v>
+      </c>
+      <c r="F189" t="s">
+        <v>80</v>
+      </c>
+      <c r="G189" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>194</v>
+      </c>
+      <c r="B190">
+        <v>133.86000000000001</v>
+      </c>
+      <c r="C190">
+        <v>54.86</v>
+      </c>
+      <c r="D190">
+        <v>180</v>
+      </c>
+      <c r="E190" t="s">
+        <v>100</v>
+      </c>
+      <c r="F190" t="s">
+        <v>101</v>
+      </c>
+      <c r="G190" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>195</v>
+      </c>
+      <c r="B191">
+        <v>133.86000000000001</v>
+      </c>
+      <c r="C191">
+        <v>30.48</v>
+      </c>
+      <c r="D191">
+        <v>180</v>
+      </c>
+      <c r="E191" t="s">
+        <v>100</v>
+      </c>
+      <c r="F191" t="s">
+        <v>101</v>
+      </c>
+      <c r="G191" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>196</v>
+      </c>
+      <c r="B192">
+        <v>133.72999999999999</v>
+      </c>
+      <c r="C192">
+        <v>79.25</v>
+      </c>
+      <c r="D192">
+        <v>180</v>
+      </c>
+      <c r="E192" t="s">
+        <v>100</v>
+      </c>
+      <c r="F192" t="s">
+        <v>101</v>
+      </c>
+      <c r="G192" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>197</v>
+      </c>
+      <c r="B193">
+        <v>150.11000000000001</v>
+      </c>
+      <c r="C193">
+        <v>54.86</v>
+      </c>
+      <c r="D193">
+        <v>180</v>
+      </c>
+      <c r="E193" t="s">
+        <v>100</v>
+      </c>
+      <c r="F193" t="s">
+        <v>101</v>
+      </c>
+      <c r="G193" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>198</v>
+      </c>
+      <c r="B194">
+        <v>150.11000000000001</v>
+      </c>
+      <c r="C194">
+        <v>30.48</v>
+      </c>
+      <c r="D194">
+        <v>180</v>
+      </c>
+      <c r="E194" t="s">
+        <v>100</v>
+      </c>
+      <c r="F194" t="s">
+        <v>101</v>
+      </c>
+      <c r="G194" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>199</v>
+      </c>
+      <c r="B195">
+        <v>149.99</v>
+      </c>
+      <c r="C195">
+        <v>79.25</v>
+      </c>
+      <c r="D195">
+        <v>180</v>
+      </c>
+      <c r="E195" t="s">
+        <v>100</v>
+      </c>
+      <c r="F195" t="s">
+        <v>101</v>
+      </c>
+      <c r="G195" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>200</v>
+      </c>
+      <c r="B196">
+        <v>166.37</v>
+      </c>
+      <c r="C196">
+        <v>54.86</v>
+      </c>
+      <c r="D196">
+        <v>180</v>
+      </c>
+      <c r="E196" t="s">
+        <v>100</v>
+      </c>
+      <c r="F196" t="s">
+        <v>101</v>
+      </c>
+      <c r="G196" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>201</v>
+      </c>
+      <c r="B197">
+        <v>166.24</v>
+      </c>
+      <c r="C197">
+        <v>79.25</v>
+      </c>
+      <c r="D197">
+        <v>180</v>
+      </c>
+      <c r="E197" t="s">
+        <v>100</v>
+      </c>
+      <c r="F197" t="s">
+        <v>101</v>
+      </c>
+      <c r="G197" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>236</v>
+      </c>
+      <c r="B198">
+        <v>60.33</v>
+      </c>
+      <c r="C198">
+        <v>26.54</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198" t="s">
+        <v>100</v>
+      </c>
+      <c r="F198" t="s">
+        <v>101</v>
+      </c>
+      <c r="G198" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>